<commit_message>
Agricultural Products Net Import Value (Import-Export): F3=(F3.1-F3.2)
</commit_message>
<xml_diff>
--- a/01_RawData/01_DomainKnowledge_01_DataPreparation.xlsx
+++ b/01_RawData/01_DomainKnowledge_01_DataPreparation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Branches\WEFN\01_RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E549287-5E33-4FAC-9D21-3A7533EB8B5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{022993DC-4C59-4335-B006-BC021297CA2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -186,10 +186,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Agricultural Products Net Import Value (Import-Export) per Capita</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>Yearly Population Increase Percentage</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -206,10 +202,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>F3=(F3.1-F3.2)/F3.3</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>https://data.worldbank.org/indicator/ER.H2O.INTR.PC</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -238,10 +230,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>F1.A</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>Kyrgyz Republic</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -255,6 +243,18 @@
   </si>
   <si>
     <t>https://data.worldbank.org/indicator/SP.POP.GROW</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1*</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>F3=(F3.1-F3.2)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agricultural Products Net Import Value (Import-Export)</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -265,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,6 +451,32 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -880,7 +906,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,6 +926,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1260,18 +1298,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.77734375" customWidth="1"/>
     <col min="9" max="12" width="8.77734375" customWidth="1"/>
@@ -1294,7 +1332,7 @@
       <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1332,11 +1370,12 @@
       <c r="E2">
         <v>313585</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>37383887</v>
       </c>
-      <c r="G2" s="4">
-        <v>0.26000913174170465</v>
+      <c r="G2" s="7">
+        <f>D2-E2</f>
+        <v>9720152</v>
       </c>
       <c r="H2" s="4">
         <v>1.95141520944077</v>
@@ -1370,11 +1409,12 @@
       <c r="E3">
         <v>20965</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="8">
         <v>25107931</v>
       </c>
-      <c r="G3" s="4">
-        <v>0.14079403834589158</v>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G37" si="0">D3-E3</f>
+        <v>3535047</v>
       </c>
       <c r="H3" s="4">
         <v>3.5977743076249902</v>
@@ -1408,11 +1448,12 @@
       <c r="E4">
         <v>293369</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>2884229</v>
       </c>
-      <c r="G4" s="4">
-        <v>0.17584942111045967</v>
+      <c r="G4" s="7">
+        <f t="shared" si="0"/>
+        <v>507190</v>
       </c>
       <c r="H4" s="4">
         <v>0.26701321436823899</v>
@@ -1446,11 +1487,12 @@
       <c r="E5">
         <v>484257</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <v>16571246</v>
       </c>
-      <c r="G5" s="4">
-        <v>-1.1020897281954537E-3</v>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>-18263</v>
       </c>
       <c r="H5" s="4">
         <v>2.9973924775883001</v>
@@ -1484,11 +1526,12 @@
       <c r="E6">
         <v>53705319</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <v>1350695000</v>
       </c>
-      <c r="G6" s="4">
-        <v>6.7322044577051071E-2</v>
+      <c r="G6" s="7">
+        <f t="shared" si="0"/>
+        <v>90931549</v>
       </c>
       <c r="H6" s="4">
         <v>0.487231117971201</v>
@@ -1522,11 +1565,12 @@
       <c r="E7">
         <v>3838195</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>4688000</v>
       </c>
-      <c r="G7" s="4">
-        <v>-0.45157081911262797</v>
+      <c r="G7" s="7">
+        <f t="shared" si="0"/>
+        <v>-2116964</v>
       </c>
       <c r="H7" s="4">
         <v>1.1782883525971199</v>
@@ -1560,11 +1604,12 @@
       <c r="E8">
         <v>2373603</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>92726971</v>
       </c>
-      <c r="G8" s="4">
-        <v>-9.6591314300560945E-3</v>
+      <c r="G8" s="7">
+        <f t="shared" si="0"/>
+        <v>-895662</v>
       </c>
       <c r="H8" s="4">
         <v>2.8296172142251699</v>
@@ -1598,11 +1643,12 @@
       <c r="E9">
         <v>2699118</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>25996449</v>
       </c>
-      <c r="G9" s="4">
-        <v>-4.3987507678452546E-2</v>
+      <c r="G9" s="7">
+        <f t="shared" si="0"/>
+        <v>-1143519</v>
       </c>
       <c r="H9" s="4">
         <v>2.3694753111338902</v>
@@ -1636,11 +1682,12 @@
       <c r="E10">
         <v>4782746</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <v>14781942</v>
       </c>
-      <c r="G10" s="4">
-        <v>-0.16795885141478703</v>
+      <c r="G10" s="7">
+        <f t="shared" si="0"/>
+        <v>-2482758</v>
       </c>
       <c r="H10" s="4">
         <v>1.77749578673149</v>
@@ -1674,11 +1721,12 @@
       <c r="E11">
         <v>38166024</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>1265782790</v>
       </c>
-      <c r="G11" s="4">
-        <v>-1.4205114133365646E-2</v>
+      <c r="G11" s="7">
+        <f t="shared" si="0"/>
+        <v>-17980589</v>
       </c>
       <c r="H11" s="4">
         <v>1.2316229280211299</v>
@@ -1712,11 +1760,12 @@
       <c r="E12">
         <v>38281998</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>248452413</v>
       </c>
-      <c r="G12" s="4">
-        <v>-8.4092972765774668E-2</v>
+      <c r="G12" s="7">
+        <f t="shared" si="0"/>
+        <v>-20893102</v>
       </c>
       <c r="H12" s="4">
         <v>1.35189219176242</v>
@@ -1750,11 +1799,12 @@
       <c r="E13">
         <v>2362798</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <v>7910500</v>
       </c>
-      <c r="G13" s="4">
-        <v>0.32708096833322797</v>
+      <c r="G13" s="7">
+        <f t="shared" si="0"/>
+        <v>2587374</v>
       </c>
       <c r="H13" s="4">
         <v>1.8461513212671099</v>
@@ -1788,11 +1838,12 @@
       <c r="E14">
         <v>40109043</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="8">
         <v>59539717</v>
       </c>
-      <c r="G14" s="4">
-        <v>8.4778938401739459E-2</v>
+      <c r="G14" s="7">
+        <f t="shared" si="0"/>
+        <v>5047714</v>
       </c>
       <c r="H14" s="4">
         <v>0.26954123952099601</v>
@@ -1826,11 +1877,12 @@
       <c r="E15">
         <v>368032</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="8">
         <v>2842132</v>
       </c>
-      <c r="G15" s="4">
-        <v>0.2190795501405283</v>
+      <c r="G15" s="7">
+        <f t="shared" si="0"/>
+        <v>622653</v>
       </c>
       <c r="H15" s="4">
         <v>0.57173146642299799</v>
@@ -1864,11 +1916,12 @@
       <c r="E16">
         <v>3287133</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="8">
         <v>127629000</v>
       </c>
-      <c r="G16" s="4">
-        <v>0.49572278243972767</v>
+      <c r="G16" s="7">
+        <f t="shared" si="0"/>
+        <v>63268603</v>
       </c>
       <c r="H16" s="4">
         <v>-0.15971067584434701</v>
@@ -1902,11 +1955,12 @@
       <c r="E17">
         <v>1370229</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="8">
         <v>8090872</v>
       </c>
-      <c r="G17" s="4">
-        <v>0.26856721994860383</v>
+      <c r="G17" s="7">
+        <f t="shared" si="0"/>
+        <v>2172943</v>
       </c>
       <c r="H17" s="4">
         <v>5.4315865678996902</v>
@@ -1940,11 +1994,12 @@
       <c r="E18">
         <v>2069926</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="8">
         <v>44343410</v>
       </c>
-      <c r="G18" s="4">
-        <v>-8.9931063037326179E-3</v>
+      <c r="G18" s="7">
+        <f t="shared" si="0"/>
+        <v>-398785</v>
       </c>
       <c r="H18" s="4">
         <v>2.6627048597740899</v>
@@ -1978,11 +2033,12 @@
       <c r="E19">
         <v>27287</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="8">
         <v>24800612</v>
       </c>
-      <c r="G19" s="4">
-        <v>2.3793324132485118E-2</v>
+      <c r="G19" s="7">
+        <f t="shared" si="0"/>
+        <v>590089</v>
       </c>
       <c r="H19" s="4">
         <v>0.51431979694602203</v>
@@ -2016,11 +2072,12 @@
       <c r="E20">
         <v>5032328</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="8">
         <v>50199853</v>
       </c>
-      <c r="G20" s="4">
-        <v>0.39476474164177333</v>
+      <c r="G20" s="7">
+        <f t="shared" si="0"/>
+        <v>19817132</v>
       </c>
       <c r="H20" s="4">
         <v>0.52571366060041402</v>
@@ -2040,7 +2097,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5">
         <v>8726.2804965044907</v>
@@ -2054,11 +2111,12 @@
       <c r="E21">
         <v>263327</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="8">
         <v>5607200</v>
       </c>
-      <c r="G21" s="4">
-        <v>9.018280068483378E-2</v>
+      <c r="G21" s="7">
+        <f t="shared" si="0"/>
+        <v>505673</v>
       </c>
       <c r="H21" s="4">
         <v>1.6652365593996199</v>
@@ -2092,11 +2150,12 @@
       <c r="E22">
         <v>614971</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="8">
         <v>5538634</v>
       </c>
-      <c r="G22" s="4">
-        <v>0.45676948503909087</v>
+      <c r="G22" s="7">
+        <f t="shared" si="0"/>
+        <v>2529879</v>
       </c>
       <c r="H22" s="4">
         <v>6.26387989274438</v>
@@ -2130,11 +2189,12 @@
       <c r="E23">
         <v>3838</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="8">
         <v>2014990</v>
       </c>
-      <c r="G23" s="4">
-        <v>0.10723824932133658</v>
+      <c r="G23" s="7">
+        <f t="shared" si="0"/>
+        <v>216084</v>
       </c>
       <c r="H23" s="4">
         <v>0.557534245861524</v>
@@ -2168,11 +2228,12 @@
       <c r="E24">
         <v>30875352</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="8">
         <v>29068159</v>
       </c>
-      <c r="G24" s="4">
-        <v>-0.41091546251690725</v>
+      <c r="G24" s="7">
+        <f t="shared" si="0"/>
+        <v>-11944556</v>
       </c>
       <c r="H24" s="4">
         <v>1.44566067334625</v>
@@ -2206,11 +2267,12 @@
       <c r="E25">
         <v>21656035</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="8">
         <v>117274155</v>
       </c>
-      <c r="G25" s="4">
-        <v>4.2578136674700409E-2</v>
+      <c r="G25" s="7">
+        <f t="shared" si="0"/>
+        <v>4993315</v>
       </c>
       <c r="H25" s="4">
         <v>1.3552892520419</v>
@@ -2245,11 +2307,12 @@
       <c r="E26">
         <v>81900</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="8">
         <v>620601</v>
       </c>
-      <c r="G26" s="4">
-        <v>0.76750762567253361</v>
+      <c r="G26" s="7">
+        <f t="shared" si="0"/>
+        <v>476316</v>
       </c>
       <c r="H26" s="4">
         <v>8.4147408002309396E-2</v>
@@ -2284,11 +2347,12 @@
       <c r="E27">
         <v>2101379</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="8">
         <v>33241898</v>
       </c>
-      <c r="G27" s="4">
-        <v>0.1092790790706355</v>
+      <c r="G27" s="7">
+        <f t="shared" si="0"/>
+        <v>3632644</v>
       </c>
       <c r="H27" s="4">
         <v>1.3936059661850999</v>
@@ -2322,11 +2386,12 @@
       <c r="E28">
         <v>237990</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="8">
         <v>26989862</v>
       </c>
-      <c r="G28" s="4">
-        <v>2.5278713911171535E-2</v>
+      <c r="G28" s="7">
+        <f t="shared" si="0"/>
+        <v>682269</v>
       </c>
       <c r="H28" s="4">
         <v>-0.19090792417970401</v>
@@ -2360,11 +2425,12 @@
       <c r="E29">
         <v>4712503</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="8">
         <v>187281475</v>
       </c>
-      <c r="G29" s="4">
-        <v>5.4482110416953942E-3</v>
+      <c r="G29" s="7">
+        <f t="shared" si="0"/>
+        <v>1020349</v>
       </c>
       <c r="H29" s="4">
         <v>2.1267117557463999</v>
@@ -2398,11 +2464,12 @@
       <c r="E30">
         <v>4203359</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="8">
         <v>29506788</v>
       </c>
-      <c r="G30" s="4">
-        <v>4.9619429942696575E-3</v>
+      <c r="G30" s="7">
+        <f t="shared" si="0"/>
+        <v>146411</v>
       </c>
       <c r="H30" s="4">
         <v>0.82513803881188197</v>
@@ -2436,11 +2503,12 @@
       <c r="E31">
         <v>8463777</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="8">
         <v>5312437</v>
       </c>
-      <c r="G31" s="4">
-        <v>0.58837629509771128</v>
+      <c r="G31" s="7">
+        <f t="shared" si="0"/>
+        <v>3125712</v>
       </c>
       <c r="H31" s="4">
         <v>2.4533903303101798</v>
@@ -2474,11 +2542,12 @@
       <c r="E32">
         <v>638248</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="8">
         <v>20442541</v>
       </c>
-      <c r="G32" s="4">
-        <v>8.7238029753737567E-2</v>
+      <c r="G32" s="7">
+        <f t="shared" si="0"/>
+        <v>1783367</v>
       </c>
       <c r="H32" s="4">
         <v>-3.0847343185318801</v>
@@ -2512,11 +2581,12 @@
       <c r="E33">
         <v>141893</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="8">
         <v>7874835</v>
       </c>
-      <c r="G33" s="4">
-        <v>6.086222758953045E-2</v>
+      <c r="G33" s="7">
+        <f t="shared" si="0"/>
+        <v>479280</v>
       </c>
       <c r="H33" s="4">
         <v>2.2775332172473699</v>
@@ -2536,7 +2606,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B34" s="5">
         <v>1785.2406124982001</v>
@@ -2550,11 +2620,12 @@
       <c r="E34">
         <v>1587723</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="8">
         <v>47052481</v>
       </c>
-      <c r="G34" s="4">
-        <v>-6.1568060566243041E-3</v>
+      <c r="G34" s="7">
+        <f t="shared" si="0"/>
+        <v>-289693</v>
       </c>
       <c r="H34" s="4">
         <v>2.9748881696736298</v>
@@ -2588,11 +2659,12 @@
       <c r="E35">
         <v>32640301</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="8">
         <v>67835957</v>
       </c>
-      <c r="G35" s="4">
-        <v>-0.32041349398225488</v>
+      <c r="G35" s="7">
+        <f t="shared" si="0"/>
+        <v>-21735556</v>
       </c>
       <c r="H35" s="4">
         <v>0.469250686880267</v>
@@ -2626,11 +2698,12 @@
       <c r="E36">
         <v>1476032</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="8">
         <v>10847002</v>
       </c>
-      <c r="G36" s="4">
-        <v>0.10909549016401029</v>
+      <c r="G36" s="7">
+        <f t="shared" si="0"/>
+        <v>1183359</v>
       </c>
       <c r="H36" s="4">
         <v>0.97386081240491396</v>
@@ -2650,7 +2723,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B37" s="5">
         <v>2276.2874505211598</v>
@@ -2664,11 +2737,12 @@
       <c r="E37">
         <v>28644375</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="8">
         <v>63700215</v>
       </c>
-      <c r="G37" s="4">
-        <v>0.49454096818982479</v>
+      <c r="G37" s="7">
+        <f t="shared" si="0"/>
+        <v>31502366</v>
       </c>
       <c r="H37" s="4">
         <v>0.69535313232226903</v>
@@ -2701,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78054FFB-0FC1-404F-8536-4A80A54A69F6}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -2730,27 +2804,27 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>2003</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2764,7 +2838,7 @@
         <v>2012</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2772,13 +2846,13 @@
         <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2786,27 +2860,27 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>2012</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="8">
         <v>2012</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>62</v>
+      <c r="D7" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2814,13 +2888,13 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>2012</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2828,13 +2902,13 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>2012</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>